<commit_message>
JS, DataViz and dataset updated
</commit_message>
<xml_diff>
--- a/02_Dataset/hadr-21-22_clean.xlsx
+++ b/02_Dataset/hadr-21-22_clean.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenae\Documents\KU Boot Camp\Repos\project3_data_viz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Data Analytics Boot Camp\Section 4 - Visualizations\Project 3\project3_data_viz\02_Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0934ABE5-243E-44E2-A13B-5551E02DFB08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4650" yWindow="-16200" windowWidth="19410" windowHeight="15585" xr2:uid="{4BFB5647-B1C0-48D7-B5BF-B8583E2E5AE1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="HADR 07-01-21 to 06-30-22" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'HADR 07-01-21 to 06-30-22'!$A$1:$AD$432</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4271,7 +4270,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4685,46 +4684,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0774DE2A-0243-434F-BFEB-08272A69030B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB432"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.21875" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="67" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="11.21875" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.44140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.21875" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.5546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.88671875" style="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.21875" style="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.88671875" style="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="12" style="13" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="8.88671875" style="1"/>
+    <col min="29" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4810,7 +4807,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>106580996</v>
       </c>
@@ -4896,7 +4893,7 @@
         <v>451166992</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>106150788</v>
       </c>
@@ -4982,7 +4979,7 @@
         <v>390366607</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>106171049</v>
       </c>
@@ -5068,7 +5065,7 @@
         <v>121827575</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>106150706</v>
       </c>
@@ -5154,7 +5151,7 @@
         <v>202162322</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>106190323</v>
       </c>
@@ -5240,7 +5237,7 @@
         <v>351175441</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>106164029</v>
       </c>
@@ -5326,7 +5323,7 @@
         <v>756273046</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>106234038</v>
       </c>
@@ -5412,7 +5409,7 @@
         <v>140974760</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>106390923</v>
       </c>
@@ -5498,7 +5495,7 @@
         <v>240345529</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>106231013</v>
       </c>
@@ -5584,7 +5581,7 @@
         <v>33410809</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>106100797</v>
       </c>
@@ -5670,7 +5667,7 @@
         <v>289898512</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>106560525</v>
       </c>
@@ -5756,7 +5753,7 @@
         <v>175402885</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>106554011</v>
       </c>
@@ -5842,7 +5839,7 @@
         <v>379691130</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>106281078</v>
       </c>
@@ -5928,7 +5925,7 @@
         <v>161588618</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>106154168</v>
       </c>
@@ -6014,7 +6011,7 @@
         <v>73029438</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>106540816</v>
       </c>
@@ -6100,7 +6097,7 @@
         <v>47090497</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>106231396</v>
       </c>
@@ -6186,7 +6183,7 @@
         <v>259016371</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>106481015</v>
       </c>
@@ -6272,7 +6269,7 @@
         <v>4214012</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>106190878</v>
       </c>
@@ -6358,7 +6355,7 @@
         <v>784724749</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>106301098</v>
       </c>
@@ -6444,7 +6441,7 @@
         <v>59970753</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>106410817</v>
       </c>
@@ -6530,7 +6527,7 @@
         <v>79012659</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>106010735</v>
       </c>
@@ -6616,7 +6613,7 @@
         <v>42355652</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>106190017</v>
       </c>
@@ -6702,7 +6699,7 @@
         <v>179078523</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>106010739</v>
       </c>
@@ -6788,7 +6785,7 @@
         <v>325330445</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>106010937</v>
       </c>
@@ -6874,7 +6871,7 @@
         <v>930756968</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>106370652</v>
       </c>
@@ -6960,7 +6957,7 @@
         <v>128517802</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>106370749</v>
       </c>
@@ -7046,7 +7043,7 @@
         <v>20187472</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>106194010</v>
       </c>
@@ -7132,7 +7129,7 @@
         <v>9615633</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>106301188</v>
       </c>
@@ -7218,7 +7215,7 @@
         <v>30890604</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>106190034</v>
       </c>
@@ -7304,7 +7301,7 @@
         <v>580183773</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>106364231</v>
       </c>
@@ -7390,7 +7387,7 @@
         <v>1013547767</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>106400683</v>
       </c>
@@ -7476,7 +7473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>106494048</v>
       </c>
@@ -7562,7 +7559,7 @@
         <v>22085431</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>106190163</v>
       </c>
@@ -7648,7 +7645,7 @@
         <v>62847461</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>106190462</v>
       </c>
@@ -7734,7 +7731,7 @@
         <v>17970648</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>106374024</v>
       </c>
@@ -7820,7 +7817,7 @@
         <v>37980274</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>106560203</v>
       </c>
@@ -7906,7 +7903,7 @@
         <v>17140742</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>106154044</v>
       </c>
@@ -7992,7 +7989,7 @@
         <v>5361771</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>106154101</v>
       </c>
@@ -8078,7 +8075,7 @@
         <v>128308993</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>106150722</v>
       </c>
@@ -8164,7 +8161,7 @@
         <v>871000367</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>106364121</v>
       </c>
@@ -8250,7 +8247,7 @@
         <v>42078967</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>106184008</v>
       </c>
@@ -8336,7 +8333,7 @@
         <v>39717311</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>106190052</v>
       </c>
@@ -8422,7 +8419,7 @@
         <v>94704934</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>106364430</v>
       </c>
@@ -8508,7 +8505,7 @@
         <v>85864226</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>106090793</v>
       </c>
@@ -8594,7 +8591,7 @@
         <v>346571160</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>106361110</v>
       </c>
@@ -8680,7 +8677,7 @@
         <v>56301605</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>106190081</v>
       </c>
@@ -8766,7 +8763,7 @@
         <v>202093483</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>106190020</v>
       </c>
@@ -8852,7 +8849,7 @@
         <v>162520400</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>106044006</v>
       </c>
@@ -8938,7 +8935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>106190125</v>
       </c>
@@ -9024,7 +9021,7 @@
         <v>776981481</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>106384202</v>
       </c>
@@ -9110,7 +9107,7 @@
         <v>1114604433</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>106384176</v>
       </c>
@@ -9196,7 +9193,7 @@
         <v>3003876902</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>106190155</v>
       </c>
@@ -9282,7 +9279,7 @@
         <v>201590718</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>106364050</v>
       </c>
@@ -9368,7 +9365,7 @@
         <v>129699976</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>106190137</v>
       </c>
@@ -9454,7 +9451,7 @@
         <v>514394249</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>106370033</v>
       </c>
@@ -9540,7 +9537,7 @@
         <v>11346511</v>
       </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>106190045</v>
       </c>
@@ -9626,7 +9623,7 @@
         <v>10225528</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>106190500</v>
       </c>
@@ -9712,7 +9709,7 @@
         <v>185230753</v>
       </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>106190555</v>
       </c>
@@ -9798,7 +9795,7 @@
         <v>8714572106</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>106190148</v>
       </c>
@@ -9884,7 +9881,7 @@
         <v>411716787</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>106105125</v>
       </c>
@@ -9970,7 +9967,7 @@
         <v>11200520</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>106500954</v>
       </c>
@@ -10056,7 +10053,7 @@
         <v>146030980</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>106301140</v>
       </c>
@@ -10142,7 +10139,7 @@
         <v>22201149</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>106434051</v>
       </c>
@@ -10228,7 +10225,7 @@
         <v>7007310</v>
       </c>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>106304113</v>
       </c>
@@ -10314,7 +10311,7 @@
         <v>61482456</v>
       </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>106190170</v>
       </c>
@@ -10400,7 +10397,7 @@
         <v>2047619181</v>
       </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>106300032</v>
       </c>
@@ -10486,7 +10483,7 @@
         <v>1509366241</v>
       </c>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>106382715</v>
       </c>
@@ -10572,7 +10569,7 @@
         <v>304914670</v>
       </c>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>106361144</v>
       </c>
@@ -10658,7 +10655,7 @@
         <v>154275297</v>
       </c>
     </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>106314029</v>
       </c>
@@ -10744,7 +10741,7 @@
         <v>930961</v>
       </c>
     </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>106190176</v>
       </c>
@@ -10830,7 +10827,7 @@
         <v>2830279706</v>
       </c>
     </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>106100005</v>
       </c>
@@ -10916,7 +10913,7 @@
         <v>814445693</v>
       </c>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>106100697</v>
       </c>
@@ -11002,7 +10999,7 @@
         <v>26038867</v>
       </c>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>106105051</v>
       </c>
@@ -11088,7 +11085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <v>106190766</v>
       </c>
@@ -11174,7 +11171,7 @@
         <v>26400941</v>
       </c>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>106190184</v>
       </c>
@@ -11260,7 +11257,7 @@
         <v>24230190</v>
       </c>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <v>106301155</v>
       </c>
@@ -11346,7 +11343,7 @@
         <v>19965959</v>
       </c>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <v>106190587</v>
       </c>
@@ -11432,7 +11429,7 @@
         <v>123336165</v>
       </c>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <v>106361458</v>
       </c>
@@ -11518,7 +11515,7 @@
         <v>13907060</v>
       </c>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <v>106060870</v>
       </c>
@@ -11604,7 +11601,7 @@
         <v>57936896</v>
       </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
         <v>106190475</v>
       </c>
@@ -11690,7 +11687,7 @@
         <v>6900820</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>106190197</v>
       </c>
@@ -11776,7 +11773,7 @@
         <v>70145505</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
         <v>106361323</v>
       </c>
@@ -11862,7 +11859,7 @@
         <v>157501736</v>
       </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>106270744</v>
       </c>
@@ -11948,7 +11945,7 @@
         <v>989631299</v>
       </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>106560473</v>
       </c>
@@ -12034,7 +12031,7 @@
         <v>973567747</v>
       </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>106100717</v>
       </c>
@@ -12120,7 +12117,7 @@
         <v>1992621410</v>
       </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>106070924</v>
       </c>
@@ -12206,7 +12203,7 @@
         <v>644524420</v>
       </c>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>106331152</v>
       </c>
@@ -12292,7 +12289,7 @@
         <v>177349652</v>
       </c>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
         <v>106154160</v>
       </c>
@@ -12378,7 +12375,7 @@
         <v>5177459</v>
       </c>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
         <v>106344170</v>
       </c>
@@ -12464,7 +12461,7 @@
         <v>8388265</v>
       </c>
     </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>106344188</v>
       </c>
@@ -12550,7 +12547,7 @@
         <v>8453335</v>
       </c>
     </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>106434220</v>
       </c>
@@ -12636,7 +12633,7 @@
         <v>7586724</v>
       </c>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
         <v>106484062</v>
       </c>
@@ -12722,7 +12719,7 @@
         <v>4750234</v>
       </c>
     </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A94" s="4">
         <v>106390846</v>
       </c>
@@ -12808,7 +12805,7 @@
         <v>96777305</v>
       </c>
     </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A95" s="4">
         <v>106190232</v>
       </c>
@@ -12894,7 +12891,7 @@
         <v>170623399</v>
       </c>
     </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A96" s="4">
         <v>106331164</v>
       </c>
@@ -12980,7 +12977,7 @@
         <v>867717476</v>
       </c>
     </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A97" s="4">
         <v>106364144</v>
       </c>
@@ -13066,7 +13063,7 @@
         <v>322283731</v>
       </c>
     </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A98" s="4">
         <v>106190681</v>
       </c>
@@ -13152,7 +13149,7 @@
         <v>18492183</v>
       </c>
     </row>
-    <row r="99" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A99" s="4">
         <v>106392287</v>
       </c>
@@ -13238,7 +13235,7 @@
         <v>137363801</v>
       </c>
     </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A100" s="4">
         <v>106331293</v>
       </c>
@@ -13324,7 +13321,7 @@
         <v>117352000</v>
       </c>
     </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A101" s="4">
         <v>106500852</v>
       </c>
@@ -13410,7 +13407,7 @@
         <v>857069604</v>
       </c>
     </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A102" s="4">
         <v>106440755</v>
       </c>
@@ -13496,7 +13493,7 @@
         <v>1008765560</v>
       </c>
     </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A103" s="4">
         <v>106190256</v>
       </c>
@@ -13582,7 +13579,7 @@
         <v>68012928</v>
       </c>
     </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A104" s="4">
         <v>106320859</v>
       </c>
@@ -13668,7 +13665,7 @@
         <v>39921243</v>
       </c>
     </row>
-    <row r="105" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A105" s="4">
         <v>106014233</v>
       </c>
@@ -13754,7 +13751,7 @@
         <v>339848567</v>
       </c>
     </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A106" s="4">
         <v>106331168</v>
       </c>
@@ -13840,7 +13837,7 @@
         <v>1205005818</v>
       </c>
     </row>
-    <row r="107" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A107" s="4">
         <v>106430763</v>
       </c>
@@ -13926,7 +13923,7 @@
         <v>3117600868</v>
       </c>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A108" s="4">
         <v>106130699</v>
       </c>
@@ -14012,7 +14009,7 @@
         <v>230555259</v>
       </c>
     </row>
-    <row r="109" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A109" s="4">
         <v>106190298</v>
       </c>
@@ -14098,7 +14095,7 @@
         <v>152542583</v>
       </c>
     </row>
-    <row r="110" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A110" s="4">
         <v>106190636</v>
       </c>
@@ -14184,7 +14181,7 @@
         <v>724490559</v>
       </c>
     </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A111" s="4">
         <v>106500867</v>
       </c>
@@ -14270,7 +14267,7 @@
         <v>257161617</v>
       </c>
     </row>
-    <row r="112" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
         <v>106190280</v>
       </c>
@@ -14356,7 +14353,7 @@
         <v>53966497</v>
       </c>
     </row>
-    <row r="113" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A113" s="4">
         <v>106154022</v>
       </c>
@@ -14442,7 +14439,7 @@
         <v>30302989</v>
       </c>
     </row>
-    <row r="114" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A114" s="4">
         <v>106504079</v>
       </c>
@@ -14528,7 +14525,7 @@
         <v>6068263</v>
       </c>
     </row>
-    <row r="115" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A115" s="4">
         <v>106334678</v>
       </c>
@@ -14614,7 +14611,7 @@
         <v>24760021</v>
       </c>
     </row>
-    <row r="116" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A116" s="4">
         <v>106040962</v>
       </c>
@@ -14700,7 +14697,7 @@
         <v>720614974</v>
       </c>
     </row>
-    <row r="117" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A117" s="4">
         <v>106474007</v>
       </c>
@@ -14786,7 +14783,7 @@
         <v>78178703</v>
       </c>
     </row>
-    <row r="118" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A118" s="4">
         <v>106301357</v>
       </c>
@@ -14872,7 +14869,7 @@
         <v>46506742</v>
       </c>
     </row>
-    <row r="119" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A119" s="4">
         <v>106301175</v>
       </c>
@@ -14958,7 +14955,7 @@
         <v>577975083</v>
       </c>
     </row>
-    <row r="120" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A120" s="4">
         <v>106014034</v>
       </c>
@@ -15044,7 +15041,7 @@
         <v>189861511</v>
       </c>
     </row>
-    <row r="121" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A121" s="4">
         <v>106400480</v>
       </c>
@@ -15130,7 +15127,7 @@
         <v>149569529</v>
       </c>
     </row>
-    <row r="122" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A122" s="4">
         <v>106104047</v>
       </c>
@@ -15216,7 +15213,7 @@
         <v>171971332</v>
       </c>
     </row>
-    <row r="123" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A123" s="4">
         <v>106301283</v>
       </c>
@@ -15302,7 +15299,7 @@
         <v>124573464</v>
       </c>
     </row>
-    <row r="124" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A124" s="4">
         <v>106190315</v>
       </c>
@@ -15388,7 +15385,7 @@
         <v>214040529</v>
       </c>
     </row>
-    <row r="125" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A125" s="4">
         <v>106190317</v>
       </c>
@@ -15474,7 +15471,7 @@
         <v>30185875</v>
       </c>
     </row>
-    <row r="126" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A126" s="4">
         <v>106270777</v>
       </c>
@@ -15560,7 +15557,7 @@
         <v>37830021</v>
       </c>
     </row>
-    <row r="127" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A127" s="4">
         <v>106190522</v>
       </c>
@@ -15646,7 +15643,7 @@
         <v>197349509</v>
       </c>
     </row>
-    <row r="128" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A128" s="4">
         <v>106420483</v>
       </c>
@@ -15732,7 +15729,7 @@
         <v>221854791</v>
       </c>
     </row>
-    <row r="129" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A129" s="4">
         <v>106150775</v>
       </c>
@@ -15818,7 +15815,7 @@
         <v>10956552</v>
       </c>
     </row>
-    <row r="130" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A130" s="4">
         <v>106190392</v>
       </c>
@@ -15904,7 +15901,7 @@
         <v>576121358</v>
       </c>
     </row>
-    <row r="131" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A131" s="4">
         <v>106430779</v>
       </c>
@@ -15990,7 +15987,7 @@
         <v>989670172</v>
       </c>
     </row>
-    <row r="132" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A132" s="4">
         <v>106190352</v>
       </c>
@@ -16076,7 +16073,7 @@
         <v>56044961</v>
       </c>
     </row>
-    <row r="133" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A133" s="4">
         <v>106350784</v>
       </c>
@@ -16162,7 +16159,7 @@
         <v>105630455</v>
       </c>
     </row>
-    <row r="134" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A134" s="4">
         <v>106490964</v>
       </c>
@@ -16248,7 +16245,7 @@
         <v>57660335</v>
       </c>
     </row>
-    <row r="135" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A135" s="4">
         <v>106331194</v>
       </c>
@@ -16334,7 +16331,7 @@
         <v>344826185</v>
       </c>
     </row>
-    <row r="136" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A136" s="4">
         <v>106190949</v>
       </c>
@@ -16420,7 +16417,7 @@
         <v>629956097</v>
       </c>
     </row>
-    <row r="137" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A137" s="4">
         <v>106344021</v>
       </c>
@@ -16506,7 +16503,7 @@
         <v>168286115</v>
       </c>
     </row>
-    <row r="138" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A138" s="4">
         <v>106362041</v>
       </c>
@@ -16592,7 +16589,7 @@
         <v>60973376</v>
       </c>
     </row>
-    <row r="139" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A139" s="4">
         <v>106010846</v>
       </c>
@@ -16678,7 +16675,7 @@
         <v>795562813</v>
       </c>
     </row>
-    <row r="140" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A140" s="4">
         <v>106301205</v>
       </c>
@@ -16764,7 +16761,7 @@
         <v>3973446911</v>
       </c>
     </row>
-    <row r="141" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A141" s="4">
         <v>106304460</v>
       </c>
@@ -16850,7 +16847,7 @@
         <v>76368251</v>
       </c>
     </row>
-    <row r="142" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A142" s="4">
         <v>106190382</v>
       </c>
@@ -16936,7 +16933,7 @@
         <v>589440938</v>
       </c>
     </row>
-    <row r="143" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A143" s="4">
         <v>106301209</v>
       </c>
@@ -17022,7 +17019,7 @@
         <v>103799639</v>
       </c>
     </row>
-    <row r="144" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A144" s="4">
         <v>106190400</v>
       </c>
@@ -17108,7 +17105,7 @@
         <v>1083567564</v>
       </c>
     </row>
-    <row r="145" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A145" s="4">
         <v>106121031</v>
       </c>
@@ -17194,7 +17191,7 @@
         <v>22746530</v>
       </c>
     </row>
-    <row r="146" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A146" s="4">
         <v>106380842</v>
       </c>
@@ -17280,7 +17277,7 @@
         <v>277497519</v>
       </c>
     </row>
-    <row r="147" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A147" s="4">
         <v>106220733</v>
       </c>
@@ -17366,7 +17363,7 @@
         <v>17015539</v>
       </c>
     </row>
-    <row r="148" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A148" s="4">
         <v>106331216</v>
       </c>
@@ -17452,7 +17449,7 @@
         <v>95950106</v>
       </c>
     </row>
-    <row r="149" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A149" s="4">
         <v>106074039</v>
       </c>
@@ -17538,7 +17535,7 @@
         <v>23329932</v>
       </c>
     </row>
-    <row r="150" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A150" s="4">
         <v>106071018</v>
       </c>
@@ -17624,7 +17621,7 @@
         <v>369766122</v>
       </c>
     </row>
-    <row r="151" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A151" s="4">
         <v>106070988</v>
       </c>
@@ -17710,7 +17707,7 @@
         <v>985774707</v>
       </c>
     </row>
-    <row r="152" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A152" s="4">
         <v>106196404</v>
       </c>
@@ -17796,7 +17793,7 @@
         <v>56859201</v>
       </c>
     </row>
-    <row r="153" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A153" s="4">
         <v>106074097</v>
       </c>
@@ -17882,7 +17879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A154" s="4">
         <v>106196035</v>
       </c>
@@ -17968,7 +17965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A155" s="4">
         <v>106196403</v>
       </c>
@@ -18054,7 +18051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A156" s="4">
         <v>106361223</v>
       </c>
@@ -18140,7 +18137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A157" s="4">
         <v>106014132</v>
       </c>
@@ -18226,7 +18223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A158" s="4">
         <v>106104062</v>
       </c>
@@ -18312,7 +18309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A159" s="4">
         <v>106190429</v>
       </c>
@@ -18398,7 +18395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A160" s="4">
         <v>106394009</v>
       </c>
@@ -18484,7 +18481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A161" s="4">
         <v>106334048</v>
       </c>
@@ -18570,7 +18567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A162" s="4">
         <v>106014326</v>
       </c>
@@ -18656,7 +18653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A163" s="4">
         <v>106304409</v>
       </c>
@@ -18742,7 +18739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A164" s="4">
         <v>106190432</v>
       </c>
@@ -18828,7 +18825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A165" s="4">
         <v>106414139</v>
       </c>
@@ -18914,7 +18911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A166" s="4">
         <v>106334025</v>
       </c>
@@ -19000,7 +18997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A167" s="4">
         <v>106314024</v>
       </c>
@@ -19086,7 +19083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A168" s="4">
         <v>106340913</v>
       </c>
@@ -19172,7 +19169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A169" s="4">
         <v>106370730</v>
       </c>
@@ -19258,7 +19255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A170" s="4">
         <v>106380857</v>
       </c>
@@ -19344,7 +19341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A171" s="4">
         <v>106431506</v>
       </c>
@@ -19430,7 +19427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A172" s="4">
         <v>106014337</v>
       </c>
@@ -19516,7 +19513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A173" s="4">
         <v>106210992</v>
       </c>
@@ -19602,7 +19599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A174" s="4">
         <v>106434153</v>
       </c>
@@ -19688,7 +19685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A175" s="4">
         <v>106494019</v>
       </c>
@@ -19774,7 +19771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A176" s="4">
         <v>106190431</v>
       </c>
@@ -19860,7 +19857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A177" s="4">
         <v>106342344</v>
       </c>
@@ -19946,7 +19943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A178" s="4">
         <v>106410806</v>
       </c>
@@ -20032,7 +20029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A179" s="4">
         <v>106484044</v>
       </c>
@@ -20118,7 +20115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A180" s="4">
         <v>106070990</v>
       </c>
@@ -20204,7 +20201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A181" s="4">
         <v>106190434</v>
       </c>
@@ -20290,7 +20287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A182" s="4">
         <v>106191450</v>
       </c>
@@ -20376,7 +20373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A183" s="4">
         <v>106480989</v>
       </c>
@@ -20462,7 +20459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A184" s="4">
         <v>106015000</v>
       </c>
@@ -20548,7 +20545,7 @@
         <v>22696943520</v>
       </c>
     </row>
-    <row r="185" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A185" s="4">
         <v>106191300</v>
       </c>
@@ -20634,7 +20631,7 @@
         <v>16720686815</v>
       </c>
     </row>
-    <row r="186" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A186" s="4">
         <v>106434218</v>
       </c>
@@ -20720,7 +20717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A187" s="4">
         <v>106540734</v>
       </c>
@@ -20806,7 +20803,7 @@
         <v>941938734</v>
       </c>
     </row>
-    <row r="188" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A188" s="4">
         <v>106194219</v>
       </c>
@@ -20892,7 +20889,7 @@
         <v>3023585904</v>
       </c>
     </row>
-    <row r="189" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A189" s="4">
         <v>106190150</v>
       </c>
@@ -20978,7 +20975,7 @@
         <v>16368137</v>
       </c>
     </row>
-    <row r="190" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A190" s="4">
         <v>106210993</v>
       </c>
@@ -21064,7 +21061,7 @@
         <v>23525524</v>
       </c>
     </row>
-    <row r="191" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A191" s="4">
         <v>106150736</v>
       </c>
@@ -21150,7 +21147,7 @@
         <v>498626134</v>
       </c>
     </row>
-    <row r="192" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A192" s="4">
         <v>106150737</v>
       </c>
@@ -21236,7 +21233,7 @@
         <v>38737343</v>
       </c>
     </row>
-    <row r="193" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A193" s="4">
         <v>106190049</v>
       </c>
@@ -21322,7 +21319,7 @@
         <v>26483151</v>
       </c>
     </row>
-    <row r="194" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A194" s="4">
         <v>106301127</v>
       </c>
@@ -21408,7 +21405,7 @@
         <v>22455850</v>
       </c>
     </row>
-    <row r="195" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A195" s="4">
         <v>106190449</v>
       </c>
@@ -21494,7 +21491,7 @@
         <v>55695972</v>
       </c>
     </row>
-    <row r="196" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A196" s="4">
         <v>106190305</v>
       </c>
@@ -21580,7 +21577,7 @@
         <v>28263816</v>
       </c>
     </row>
-    <row r="197" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A197" s="4">
         <v>106361274</v>
       </c>
@@ -21666,7 +21663,7 @@
         <v>51843311</v>
       </c>
     </row>
-    <row r="198" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A198" s="4">
         <v>106190599</v>
       </c>
@@ -21752,7 +21749,7 @@
         <v>40360564</v>
       </c>
     </row>
-    <row r="199" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A199" s="4">
         <v>106364188</v>
       </c>
@@ -21838,7 +21835,7 @@
         <v>11390864</v>
       </c>
     </row>
-    <row r="200" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A200" s="4">
         <v>106332172</v>
       </c>
@@ -21924,7 +21921,7 @@
         <v>11491221</v>
       </c>
     </row>
-    <row r="201" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A201" s="4">
         <v>106370721</v>
       </c>
@@ -22010,7 +22007,7 @@
         <v>22491024</v>
       </c>
     </row>
-    <row r="202" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A202" s="4">
         <v>106010887</v>
       </c>
@@ -22096,7 +22093,7 @@
         <v>30492999</v>
       </c>
     </row>
-    <row r="203" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A203" s="4">
         <v>106190196</v>
       </c>
@@ -22182,7 +22179,7 @@
         <v>19442156</v>
       </c>
     </row>
-    <row r="204" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A204" s="4">
         <v>106301380</v>
       </c>
@@ -22268,7 +22265,7 @@
         <v>42708844</v>
       </c>
     </row>
-    <row r="205" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A205" s="4">
         <v>106190661</v>
       </c>
@@ -22354,7 +22351,7 @@
         <v>69554351</v>
       </c>
     </row>
-    <row r="206" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A206" s="4">
         <v>106194981</v>
       </c>
@@ -22440,7 +22437,7 @@
         <v>1249902</v>
       </c>
     </row>
-    <row r="207" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A207" s="4">
         <v>106301234</v>
       </c>
@@ -22526,7 +22523,7 @@
         <v>77006615</v>
       </c>
     </row>
-    <row r="208" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A208" s="4">
         <v>106191227</v>
       </c>
@@ -22612,7 +22609,7 @@
         <v>2599378921</v>
       </c>
     </row>
-    <row r="209" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A209" s="4">
         <v>106191231</v>
       </c>
@@ -22698,7 +22695,7 @@
         <v>1139648389</v>
       </c>
     </row>
-    <row r="210" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A210" s="4">
         <v>106191306</v>
       </c>
@@ -22784,7 +22781,7 @@
         <v>1238400095</v>
       </c>
     </row>
-    <row r="211" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A211" s="4">
         <v>106191228</v>
       </c>
@@ -22870,7 +22867,7 @@
         <v>2862836452</v>
       </c>
     </row>
-    <row r="212" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A212" s="4">
         <v>106380865</v>
       </c>
@@ -22956,7 +22953,7 @@
         <v>643674454</v>
       </c>
     </row>
-    <row r="213" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A213" s="4">
         <v>106304583</v>
       </c>
@@ -23042,7 +23039,7 @@
         <v>15649733</v>
       </c>
     </row>
-    <row r="214" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A214" s="4">
         <v>106190240</v>
       </c>
@@ -23128,7 +23125,7 @@
         <v>294912484</v>
       </c>
     </row>
-    <row r="215" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A215" s="4">
         <v>106380868</v>
       </c>
@@ -23214,7 +23211,7 @@
         <v>37795734</v>
       </c>
     </row>
-    <row r="216" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A216" s="4">
         <v>106364014</v>
       </c>
@@ -23300,7 +23297,7 @@
         <v>40574575</v>
       </c>
     </row>
-    <row r="217" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A217" s="4">
         <v>106364502</v>
       </c>
@@ -23386,7 +23383,7 @@
         <v>1566782636</v>
       </c>
     </row>
-    <row r="218" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A218" s="4">
         <v>106361246</v>
       </c>
@@ -23472,7 +23469,7 @@
         <v>4089849527</v>
       </c>
     </row>
-    <row r="219" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A219" s="4">
         <v>106334589</v>
       </c>
@@ -23558,7 +23555,7 @@
         <v>354201453</v>
       </c>
     </row>
-    <row r="220" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A220" s="4">
         <v>106420491</v>
       </c>
@@ -23644,7 +23641,7 @@
         <v>148584613</v>
       </c>
     </row>
-    <row r="221" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A221" s="4">
         <v>106301248</v>
       </c>
@@ -23730,7 +23727,7 @@
         <v>220188034</v>
       </c>
     </row>
-    <row r="222" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A222" s="4">
         <v>106190198</v>
       </c>
@@ -23816,7 +23813,7 @@
         <v>656609492</v>
       </c>
     </row>
-    <row r="223" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A223" s="4">
         <v>106560492</v>
       </c>
@@ -23902,7 +23899,7 @@
         <v>1610972260</v>
       </c>
     </row>
-    <row r="224" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A224" s="4">
         <v>106434040</v>
       </c>
@@ -23988,7 +23985,7 @@
         <v>3584700291</v>
       </c>
     </row>
-    <row r="225" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A225" s="4">
         <v>106121002</v>
       </c>
@@ -24074,7 +24071,7 @@
         <v>41563723</v>
       </c>
     </row>
-    <row r="226" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A226" s="4">
         <v>106201281</v>
       </c>
@@ -24160,7 +24157,7 @@
         <v>81963115</v>
       </c>
     </row>
-    <row r="227" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A227" s="4">
         <v>106260011</v>
       </c>
@@ -24246,7 +24243,7 @@
         <v>189282151</v>
       </c>
     </row>
-    <row r="228" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A228" s="4">
         <v>106420493</v>
       </c>
@@ -24332,7 +24329,7 @@
         <v>527879774</v>
       </c>
     </row>
-    <row r="229" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A229" s="4">
         <v>106244027</v>
       </c>
@@ -24418,7 +24415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A230" s="4">
         <v>106211006</v>
       </c>
@@ -24504,7 +24501,7 @@
         <v>552164711</v>
       </c>
     </row>
-    <row r="231" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A231" s="4">
         <v>106050932</v>
       </c>
@@ -24590,7 +24587,7 @@
         <v>53841385</v>
       </c>
     </row>
-    <row r="232" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A232" s="4">
         <v>106090933</v>
       </c>
@@ -24676,7 +24673,7 @@
         <v>353726329</v>
       </c>
     </row>
-    <row r="233" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A233" s="4">
         <v>106191230</v>
       </c>
@@ -24762,7 +24759,7 @@
         <v>568412226</v>
       </c>
     </row>
-    <row r="234" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A234" s="4">
         <v>106450936</v>
       </c>
@@ -24848,7 +24845,7 @@
         <v>64506553</v>
       </c>
     </row>
-    <row r="235" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A235" s="4">
         <v>106240924</v>
       </c>
@@ -24934,7 +24931,7 @@
         <v>36288100</v>
       </c>
     </row>
-    <row r="236" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A236" s="4">
         <v>106500939</v>
       </c>
@@ -25020,7 +25017,7 @@
         <v>342352151</v>
       </c>
     </row>
-    <row r="237" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A237" s="4">
         <v>106190521</v>
       </c>
@@ -25106,7 +25103,7 @@
         <v>200539176</v>
       </c>
     </row>
-    <row r="238" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A238" s="4">
         <v>106190525</v>
       </c>
@@ -25192,7 +25189,7 @@
         <v>1607086846</v>
       </c>
     </row>
-    <row r="239" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A239" s="4">
         <v>106196168</v>
       </c>
@@ -25278,7 +25275,7 @@
         <v>332363140</v>
       </c>
     </row>
-    <row r="240" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A240" s="4">
         <v>106300225</v>
       </c>
@@ -25364,7 +25361,7 @@
         <v>347745146</v>
       </c>
     </row>
-    <row r="241" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A241" s="4">
         <v>106301317</v>
       </c>
@@ -25450,7 +25447,7 @@
         <v>765415247</v>
       </c>
     </row>
-    <row r="242" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A242" s="4">
         <v>106334018</v>
       </c>
@@ -25536,7 +25533,7 @@
         <v>19885343</v>
       </c>
     </row>
-    <row r="243" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A243" s="4">
         <v>106340947</v>
       </c>
@@ -25622,7 +25619,7 @@
         <v>586640136</v>
       </c>
     </row>
-    <row r="244" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A244" s="4">
         <v>106150761</v>
       </c>
@@ -25708,7 +25705,7 @@
         <v>478001342</v>
       </c>
     </row>
-    <row r="245" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A245" s="4">
         <v>106344029</v>
       </c>
@@ -25794,7 +25791,7 @@
         <v>707337933</v>
       </c>
     </row>
-    <row r="246" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A246" s="4">
         <v>106240942</v>
       </c>
@@ -25880,7 +25877,7 @@
         <v>468734791</v>
       </c>
     </row>
-    <row r="247" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A247" s="4">
         <v>106470871</v>
       </c>
@@ -25966,7 +25963,7 @@
         <v>79452492</v>
       </c>
     </row>
-    <row r="248" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A248" s="4">
         <v>106450949</v>
       </c>
@@ -26052,7 +26049,7 @@
         <v>1337633513</v>
       </c>
     </row>
-    <row r="249" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A249" s="4">
         <v>106340950</v>
       </c>
@@ -26138,7 +26135,7 @@
         <v>523952081</v>
       </c>
     </row>
-    <row r="250" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A250" s="4">
         <v>106013687</v>
       </c>
@@ -26224,7 +26221,7 @@
         <v>1086942</v>
       </c>
     </row>
-    <row r="251" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A251" s="4">
         <v>106340951</v>
       </c>
@@ -26310,7 +26307,7 @@
         <v>186750444</v>
       </c>
     </row>
-    <row r="252" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A252" s="4">
         <v>106190529</v>
       </c>
@@ -26396,7 +26393,7 @@
         <v>618751334</v>
       </c>
     </row>
-    <row r="253" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A253" s="4">
         <v>106190958</v>
       </c>
@@ -26482,7 +26479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A254" s="4">
         <v>106410852</v>
       </c>
@@ -26568,7 +26565,7 @@
         <v>593710204</v>
       </c>
     </row>
-    <row r="255" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A255" s="4">
         <v>106190524</v>
       </c>
@@ -26654,7 +26651,7 @@
         <v>98985250</v>
       </c>
     </row>
-    <row r="256" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A256" s="4">
         <v>106254005</v>
       </c>
@@ -26740,7 +26737,7 @@
         <v>90908173</v>
       </c>
     </row>
-    <row r="257" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A257" s="4">
         <v>106190541</v>
       </c>
@@ -26826,7 +26823,7 @@
         <v>15596047</v>
       </c>
     </row>
-    <row r="258" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A258" s="4">
         <v>106361166</v>
       </c>
@@ -26912,7 +26909,7 @@
         <v>125524253</v>
       </c>
     </row>
-    <row r="259" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A259" s="4">
         <v>106190547</v>
       </c>
@@ -26998,7 +26995,7 @@
         <v>76250656</v>
       </c>
     </row>
-    <row r="260" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A260" s="4">
         <v>106190552</v>
       </c>
@@ -27084,7 +27081,7 @@
         <v>127765662</v>
       </c>
     </row>
-    <row r="261" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A261" s="4">
         <v>106361266</v>
       </c>
@@ -27170,7 +27167,7 @@
         <v>60746702</v>
       </c>
     </row>
-    <row r="262" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A262" s="4">
         <v>106281266</v>
       </c>
@@ -27256,7 +27253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A263" s="4">
         <v>106274043</v>
       </c>
@@ -27342,7 +27339,7 @@
         <v>495658888</v>
       </c>
     </row>
-    <row r="264" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A264" s="4">
         <v>106301304</v>
       </c>
@@ -27428,7 +27425,7 @@
         <v>526190</v>
       </c>
     </row>
-    <row r="265" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A265" s="4">
         <v>106514033</v>
       </c>
@@ -27514,7 +27511,7 @@
         <v>1245697</v>
       </c>
     </row>
-    <row r="266" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A266" s="4">
         <v>106481357</v>
       </c>
@@ -27600,7 +27597,7 @@
         <v>886662508</v>
       </c>
     </row>
-    <row r="267" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A267" s="4">
         <v>106141273</v>
       </c>
@@ -27686,7 +27683,7 @@
         <v>163553408</v>
       </c>
     </row>
-    <row r="268" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A268" s="4">
         <v>106190568</v>
       </c>
@@ -27772,7 +27769,7 @@
         <v>540239253</v>
       </c>
     </row>
-    <row r="269" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A269" s="4">
         <v>106214034</v>
       </c>
@@ -27858,7 +27855,7 @@
         <v>50467071</v>
       </c>
     </row>
-    <row r="270" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A270" s="4">
         <v>106500967</v>
       </c>
@@ -27944,7 +27941,7 @@
         <v>122961548</v>
       </c>
     </row>
-    <row r="271" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A271" s="4">
         <v>106198495</v>
       </c>
@@ -28030,7 +28027,7 @@
         <v>15391093</v>
       </c>
     </row>
-    <row r="272" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A272" s="4">
         <v>106560501</v>
       </c>
@@ -28116,7 +28113,7 @@
         <v>40881496</v>
       </c>
     </row>
-    <row r="273" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A273" s="4">
         <v>106301566</v>
       </c>
@@ -28202,7 +28199,7 @@
         <v>113892089</v>
       </c>
     </row>
-    <row r="274" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A274" s="4">
         <v>106040802</v>
       </c>
@@ -28288,7 +28285,7 @@
         <v>15903775</v>
       </c>
     </row>
-    <row r="275" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A275" s="4">
         <v>106040937</v>
       </c>
@@ -28374,7 +28371,7 @@
         <v>519632480</v>
       </c>
     </row>
-    <row r="276" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A276" s="4">
         <v>106331226</v>
       </c>
@@ -28460,7 +28457,7 @@
         <v>24855680</v>
       </c>
     </row>
-    <row r="277" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A277" s="4">
         <v>106190696</v>
       </c>
@@ -28546,7 +28543,7 @@
         <v>84563297</v>
       </c>
     </row>
-    <row r="278" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A278" s="4">
         <v>106196405</v>
       </c>
@@ -28632,7 +28629,7 @@
         <v>243261012</v>
       </c>
     </row>
-    <row r="279" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A279" s="4">
         <v>106331288</v>
       </c>
@@ -28718,7 +28715,7 @@
         <v>21568654</v>
       </c>
     </row>
-    <row r="280" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A280" s="4">
         <v>106374382</v>
       </c>
@@ -28804,7 +28801,7 @@
         <v>7218316961</v>
       </c>
     </row>
-    <row r="281" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A281" s="4">
         <v>106370977</v>
       </c>
@@ -28890,7 +28887,7 @@
         <v>1983191686</v>
       </c>
     </row>
-    <row r="282" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A282" s="4">
         <v>106370759</v>
       </c>
@@ -28976,7 +28973,7 @@
         <v>116860069</v>
       </c>
     </row>
-    <row r="283" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A283" s="4">
         <v>106454013</v>
       </c>
@@ -29062,7 +29059,7 @@
         <v>2608414</v>
       </c>
     </row>
-    <row r="284" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A284" s="4">
         <v>106361768</v>
       </c>
@@ -29148,7 +29145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A285" s="4">
         <v>106491001</v>
       </c>
@@ -29234,7 +29231,7 @@
         <v>103958463</v>
       </c>
     </row>
-    <row r="286" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A286" s="4">
         <v>106190243</v>
       </c>
@@ -29320,7 +29317,7 @@
         <v>167649889</v>
       </c>
     </row>
-    <row r="287" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A287" s="4">
         <v>106130760</v>
       </c>
@@ -29406,7 +29403,7 @@
         <v>102250988</v>
       </c>
     </row>
-    <row r="288" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A288" s="4">
         <v>106301297</v>
       </c>
@@ -29492,7 +29489,7 @@
         <v>193661166</v>
       </c>
     </row>
-    <row r="289" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A289" s="4">
         <v>106320986</v>
       </c>
@@ -29578,7 +29575,7 @@
         <v>32436642</v>
       </c>
     </row>
-    <row r="290" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A290" s="4">
         <v>106190630</v>
       </c>
@@ -29664,7 +29661,7 @@
         <v>763775791</v>
       </c>
     </row>
-    <row r="291" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A291" s="4">
         <v>106541123</v>
       </c>
@@ -29750,7 +29747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A292" s="4">
         <v>106190631</v>
       </c>
@@ -29836,7 +29833,7 @@
         <v>1740347396</v>
       </c>
     </row>
-    <row r="293" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A293" s="4">
         <v>106361343</v>
       </c>
@@ -29922,7 +29919,7 @@
         <v>611156049</v>
       </c>
     </row>
-    <row r="294" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A294" s="4">
         <v>106190385</v>
       </c>
@@ -30008,7 +30005,7 @@
         <v>440321744</v>
       </c>
     </row>
-    <row r="295" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A295" s="4">
         <v>106190680</v>
       </c>
@@ -30094,7 +30091,7 @@
         <v>118434969</v>
       </c>
     </row>
-    <row r="296" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A296" s="4">
         <v>106190470</v>
       </c>
@@ -30180,7 +30177,7 @@
         <v>296708799</v>
       </c>
     </row>
-    <row r="297" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A297" s="4">
         <v>106301262</v>
       </c>
@@ -30266,7 +30263,7 @@
         <v>707604622</v>
       </c>
     </row>
-    <row r="298" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A298" s="4">
         <v>106281047</v>
       </c>
@@ -30352,7 +30349,7 @@
         <v>439496419</v>
       </c>
     </row>
-    <row r="299" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A299" s="4">
         <v>106121051</v>
       </c>
@@ -30438,7 +30435,7 @@
         <v>168908650</v>
       </c>
     </row>
-    <row r="300" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A300" s="4">
         <v>106491064</v>
       </c>
@@ -30524,7 +30521,7 @@
         <v>581650528</v>
       </c>
     </row>
-    <row r="301" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A301" s="4">
         <v>106190756</v>
       </c>
@@ -30610,7 +30607,7 @@
         <v>655559137</v>
       </c>
     </row>
-    <row r="302" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A302" s="4">
         <v>106301340</v>
       </c>
@@ -30696,7 +30693,7 @@
         <v>922917997</v>
       </c>
     </row>
-    <row r="303" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A303" s="4">
         <v>106121080</v>
       </c>
@@ -30782,7 +30779,7 @@
         <v>324738368</v>
       </c>
     </row>
-    <row r="304" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A304" s="4">
         <v>106190758</v>
       </c>
@@ -30868,7 +30865,7 @@
         <v>400325512</v>
       </c>
     </row>
-    <row r="305" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A305" s="4">
         <v>106301342</v>
       </c>
@@ -30954,7 +30951,7 @@
         <v>1117041775</v>
       </c>
     </row>
-    <row r="306" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A306" s="4">
         <v>106190517</v>
       </c>
@@ -31040,7 +31037,7 @@
         <v>727437119</v>
       </c>
     </row>
-    <row r="307" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A307" s="4">
         <v>106370673</v>
       </c>
@@ -31126,7 +31123,7 @@
         <v>3259665996</v>
       </c>
     </row>
-    <row r="308" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A308" s="4">
         <v>106361308</v>
       </c>
@@ -31212,7 +31209,7 @@
         <v>575689066</v>
       </c>
     </row>
-    <row r="309" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A309" s="4">
         <v>106430705</v>
       </c>
@@ -31298,7 +31295,7 @@
         <v>398882734</v>
       </c>
     </row>
-    <row r="310" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A310" s="4">
         <v>106190930</v>
       </c>
@@ -31384,7 +31381,7 @@
         <v>78627274</v>
       </c>
     </row>
-    <row r="311" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A311" s="4">
         <v>106454068</v>
       </c>
@@ -31470,7 +31467,7 @@
         <v>1021457</v>
       </c>
     </row>
-    <row r="312" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A312" s="4">
         <v>106524017</v>
       </c>
@@ -31556,7 +31553,7 @@
         <v>1074201</v>
       </c>
     </row>
-    <row r="313" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A313" s="4">
         <v>106150782</v>
       </c>
@@ -31642,7 +31639,7 @@
         <v>182576013</v>
       </c>
     </row>
-    <row r="314" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A314" s="4">
         <v>106331312</v>
       </c>
@@ -31728,7 +31725,7 @@
         <v>1539860000</v>
       </c>
     </row>
-    <row r="315" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A315" s="4">
         <v>106334487</v>
       </c>
@@ -31814,7 +31811,7 @@
         <v>863970567</v>
       </c>
     </row>
-    <row r="316" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A316" s="4">
         <v>106190796</v>
       </c>
@@ -31900,7 +31897,7 @@
         <v>5137884145</v>
       </c>
     </row>
-    <row r="317" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A317" s="4">
         <v>106344011</v>
       </c>
@@ -31986,7 +31983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A318" s="4">
         <v>106270875</v>
       </c>
@@ -32072,7 +32069,7 @@
         <v>1076073719</v>
       </c>
     </row>
-    <row r="319" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A319" s="4">
         <v>106361318</v>
       </c>
@@ -32158,7 +32155,7 @@
         <v>729122263</v>
       </c>
     </row>
-    <row r="320" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A320" s="4">
         <v>106374055</v>
       </c>
@@ -32244,7 +32241,7 @@
         <v>129458655</v>
       </c>
     </row>
-    <row r="321" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A321" s="4">
         <v>106190673</v>
       </c>
@@ -32330,7 +32327,7 @@
         <v>49293057</v>
       </c>
     </row>
-    <row r="322" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A322" s="4">
         <v>106190200</v>
       </c>
@@ -32416,7 +32413,7 @@
         <v>77776400</v>
       </c>
     </row>
-    <row r="323" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A323" s="4">
         <v>106331326</v>
       </c>
@@ -32502,7 +32499,7 @@
         <v>113846353</v>
       </c>
     </row>
-    <row r="324" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A324" s="4">
         <v>106394003</v>
       </c>
@@ -32588,7 +32585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A325" s="4">
         <v>106391010</v>
       </c>
@@ -32674,7 +32671,7 @@
         <v>596839345</v>
       </c>
     </row>
-    <row r="326" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A326" s="4">
         <v>106104023</v>
       </c>
@@ -32760,7 +32757,7 @@
         <v>12020759</v>
       </c>
     </row>
-    <row r="327" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A327" s="4">
         <v>106434032</v>
       </c>
@@ -32846,7 +32843,7 @@
         <v>56342883</v>
       </c>
     </row>
-    <row r="328" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A328" s="4">
         <v>106404046</v>
       </c>
@@ -32932,7 +32929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A329" s="4">
         <v>106410782</v>
       </c>
@@ -33018,7 +33015,7 @@
         <v>372015508</v>
       </c>
     </row>
-    <row r="330" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A330" s="4">
         <v>106074017</v>
       </c>
@@ -33104,7 +33101,7 @@
         <v>316451842</v>
       </c>
     </row>
-    <row r="331" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A331" s="4">
         <v>106420514</v>
       </c>
@@ -33190,7 +33187,7 @@
         <v>2134850221</v>
       </c>
     </row>
-    <row r="332" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A332" s="4">
         <v>106424002</v>
       </c>
@@ -33276,7 +33273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A333" s="4">
         <v>106430883</v>
       </c>
@@ -33362,7 +33359,7 @@
         <v>1038817654</v>
       </c>
     </row>
-    <row r="334" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A334" s="4">
         <v>106190687</v>
       </c>
@@ -33448,7 +33445,7 @@
         <v>1537866390</v>
       </c>
     </row>
-    <row r="335" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A335" s="4">
         <v>106420522</v>
       </c>
@@ -33534,7 +33531,7 @@
         <v>74746428</v>
       </c>
     </row>
-    <row r="336" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A336" s="4">
         <v>106371256</v>
       </c>
@@ -33620,7 +33617,7 @@
         <v>1236556794</v>
       </c>
     </row>
-    <row r="337" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A337" s="4">
         <v>106371394</v>
       </c>
@@ -33706,7 +33703,7 @@
         <v>401607650</v>
       </c>
     </row>
-    <row r="338" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A338" s="4">
         <v>106370771</v>
       </c>
@@ -33792,7 +33789,7 @@
         <v>1723640784</v>
       </c>
     </row>
-    <row r="339" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A339" s="4">
         <v>106370744</v>
       </c>
@@ -33878,7 +33875,7 @@
         <v>599548870</v>
       </c>
     </row>
-    <row r="340" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A340" s="4">
         <v>106374094</v>
       </c>
@@ -33964,7 +33961,7 @@
         <v>49539661</v>
       </c>
     </row>
-    <row r="341" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A341" s="4">
         <v>106124004</v>
       </c>
@@ -34050,7 +34047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A342" s="4">
         <v>106321016</v>
       </c>
@@ -34136,7 +34133,7 @@
         <v>20818601</v>
       </c>
     </row>
-    <row r="343" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A343" s="4">
         <v>106410891</v>
       </c>
@@ -34222,7 +34219,7 @@
         <v>541662860</v>
       </c>
     </row>
-    <row r="344" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A344" s="4">
         <v>106370875</v>
       </c>
@@ -34308,7 +34305,7 @@
         <v>734278189</v>
       </c>
     </row>
-    <row r="345" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A345" s="4">
         <v>106370689</v>
       </c>
@@ -34394,7 +34391,7 @@
         <v>180166552</v>
       </c>
     </row>
-    <row r="346" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A346" s="4">
         <v>106370714</v>
       </c>
@@ -34480,7 +34477,7 @@
         <v>1423239892</v>
       </c>
     </row>
-    <row r="347" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A347" s="4">
         <v>106374049</v>
       </c>
@@ -34566,7 +34563,7 @@
         <v>17195332</v>
       </c>
     </row>
-    <row r="348" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A348" s="4">
         <v>106370694</v>
       </c>
@@ -34652,7 +34649,7 @@
         <v>3616073701</v>
       </c>
     </row>
-    <row r="349" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A349" s="4">
         <v>106370745</v>
       </c>
@@ -34738,7 +34735,7 @@
         <v>239883608</v>
       </c>
     </row>
-    <row r="350" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A350" s="4">
         <v>106450940</v>
       </c>
@@ -34824,7 +34821,7 @@
         <v>142022460</v>
       </c>
     </row>
-    <row r="351" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A351" s="4">
         <v>106190708</v>
       </c>
@@ -34910,7 +34907,7 @@
         <v>187922016</v>
       </c>
     </row>
-    <row r="352" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A352" s="4">
         <v>106344114</v>
       </c>
@@ -34996,7 +34993,7 @@
         <v>70873868</v>
       </c>
     </row>
-    <row r="353" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A353" s="4">
         <v>106291023</v>
       </c>
@@ -35082,7 +35079,7 @@
         <v>321148641</v>
       </c>
     </row>
-    <row r="354" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A354" s="4">
         <v>106540798</v>
       </c>
@@ -35168,7 +35165,7 @@
         <v>341834422</v>
       </c>
     </row>
-    <row r="355" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A355" s="4">
         <v>106342392</v>
       </c>
@@ -35254,7 +35251,7 @@
         <v>164060124</v>
       </c>
     </row>
-    <row r="356" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A356" s="4">
         <v>106400524</v>
       </c>
@@ -35340,7 +35337,7 @@
         <v>312176517</v>
       </c>
     </row>
-    <row r="357" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A357" s="4">
         <v>106491338</v>
       </c>
@@ -35426,7 +35423,7 @@
         <v>23725013</v>
       </c>
     </row>
-    <row r="358" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A358" s="4">
         <v>106491076</v>
       </c>
@@ -35512,7 +35509,7 @@
         <v>83985450</v>
       </c>
     </row>
-    <row r="359" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A359" s="4">
         <v>106301258</v>
       </c>
@@ -35598,7 +35595,7 @@
         <v>18411292</v>
       </c>
     </row>
-    <row r="360" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A360" s="4">
         <v>106190380</v>
       </c>
@@ -35684,7 +35681,7 @@
         <v>328818830</v>
       </c>
     </row>
-    <row r="361" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A361" s="4">
         <v>106141338</v>
       </c>
@@ -35770,7 +35767,7 @@
         <v>9965578</v>
       </c>
     </row>
-    <row r="362" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A362" s="4">
         <v>106334068</v>
       </c>
@@ -35856,7 +35853,7 @@
         <v>562194935</v>
       </c>
     </row>
-    <row r="363" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A363" s="4">
         <v>106100899</v>
       </c>
@@ -35942,7 +35939,7 @@
         <v>722419355</v>
       </c>
     </row>
-    <row r="364" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A364" s="4">
         <v>106361339</v>
       </c>
@@ -36028,7 +36025,7 @@
         <v>286704169</v>
       </c>
     </row>
-    <row r="365" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A365" s="4">
         <v>106521041</v>
       </c>
@@ -36114,7 +36111,7 @@
         <v>328887638</v>
       </c>
     </row>
-    <row r="366" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A366" s="4">
         <v>106190754</v>
       </c>
@@ -36200,7 +36197,7 @@
         <v>769643422</v>
       </c>
     </row>
-    <row r="367" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A367" s="4">
         <v>106380960</v>
       </c>
@@ -36286,7 +36283,7 @@
         <v>200941038</v>
       </c>
     </row>
-    <row r="368" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A368" s="4">
         <v>106560529</v>
       </c>
@@ -36372,7 +36369,7 @@
         <v>537283103</v>
       </c>
     </row>
-    <row r="369" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A369" s="4">
         <v>106392232</v>
       </c>
@@ -36458,7 +36455,7 @@
         <v>9656180</v>
       </c>
     </row>
-    <row r="370" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A370" s="4">
         <v>106391042</v>
       </c>
@@ -36544,7 +36541,7 @@
         <v>758245716</v>
       </c>
     </row>
-    <row r="371" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A371" s="4">
         <v>106190053</v>
       </c>
@@ -36630,7 +36627,7 @@
         <v>288859694</v>
       </c>
     </row>
-    <row r="372" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A372" s="4">
         <v>106380965</v>
       </c>
@@ -36716,7 +36713,7 @@
         <v>258429588</v>
       </c>
     </row>
-    <row r="373" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A373" s="4">
         <v>106010967</v>
       </c>
@@ -36802,7 +36799,7 @@
         <v>71008486</v>
       </c>
     </row>
-    <row r="374" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A374" s="4">
         <v>106514005</v>
       </c>
@@ -36888,7 +36885,7 @@
         <v>1072329</v>
       </c>
     </row>
-    <row r="375" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A375" s="4">
         <v>106430905</v>
       </c>
@@ -36974,7 +36971,7 @@
         <v>10339511381</v>
       </c>
     </row>
-    <row r="376" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A376" s="4">
         <v>106504038</v>
       </c>
@@ -37060,7 +37057,7 @@
         <v>41270922</v>
       </c>
     </row>
-    <row r="377" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A377" s="4">
         <v>106194967</v>
       </c>
@@ -37146,7 +37143,7 @@
         <v>26762242</v>
       </c>
     </row>
-    <row r="378" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A378" s="4">
         <v>106250955</v>
       </c>
@@ -37232,7 +37229,7 @@
         <v>8265237</v>
       </c>
     </row>
-    <row r="379" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A379" s="4">
         <v>106514001</v>
       </c>
@@ -37318,7 +37315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A380" s="4">
         <v>106034002</v>
       </c>
@@ -37404,7 +37401,7 @@
         <v>64083426</v>
       </c>
     </row>
-    <row r="381" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A381" s="4">
         <v>106310791</v>
       </c>
@@ -37490,7 +37487,7 @@
         <v>66117911</v>
       </c>
     </row>
-    <row r="382" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A382" s="4">
         <v>106344017</v>
       </c>
@@ -37576,7 +37573,7 @@
         <v>16759505</v>
       </c>
     </row>
-    <row r="383" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A383" s="4">
         <v>106084001</v>
       </c>
@@ -37662,7 +37659,7 @@
         <v>47113490</v>
       </c>
     </row>
-    <row r="384" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A384" s="4">
         <v>106574010</v>
       </c>
@@ -37748,7 +37745,7 @@
         <v>78015693</v>
       </c>
     </row>
-    <row r="385" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A385" s="4">
         <v>106070934</v>
       </c>
@@ -37834,7 +37831,7 @@
         <v>121275676</v>
       </c>
     </row>
-    <row r="386" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A386" s="4">
         <v>106171395</v>
       </c>
@@ -37920,7 +37917,7 @@
         <v>47360982</v>
       </c>
     </row>
-    <row r="387" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A387" s="4">
         <v>106444012</v>
       </c>
@@ -38006,7 +38003,7 @@
         <v>41780569</v>
       </c>
     </row>
-    <row r="388" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A388" s="4">
         <v>106341051</v>
       </c>
@@ -38092,7 +38089,7 @@
         <v>1216747268</v>
       </c>
     </row>
-    <row r="389" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A389" s="4">
         <v>106311000</v>
       </c>
@@ -38178,7 +38175,7 @@
         <v>543299683</v>
       </c>
     </row>
-    <row r="390" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A390" s="4">
         <v>106494106</v>
       </c>
@@ -38264,7 +38261,7 @@
         <v>421525247</v>
       </c>
     </row>
-    <row r="391" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A391" s="4">
         <v>106481094</v>
       </c>
@@ -38350,7 +38347,7 @@
         <v>77242482</v>
       </c>
     </row>
-    <row r="392" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A392" s="4">
         <v>106514030</v>
       </c>
@@ -38436,7 +38433,7 @@
         <v>18971647</v>
       </c>
     </row>
-    <row r="393" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A393" s="4">
         <v>106391056</v>
       </c>
@@ -38522,7 +38519,7 @@
         <v>83720944</v>
       </c>
     </row>
-    <row r="394" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A394" s="4">
         <v>106291053</v>
       </c>
@@ -38608,7 +38605,7 @@
         <v>417218875</v>
       </c>
     </row>
-    <row r="395" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A395" s="4">
         <v>106190782</v>
       </c>
@@ -38694,7 +38691,7 @@
         <v>72679853</v>
       </c>
     </row>
-    <row r="396" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A396" s="4">
         <v>106094002</v>
       </c>
@@ -38780,7 +38777,7 @@
         <v>2536656</v>
       </c>
     </row>
-    <row r="397" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A397" s="4">
         <v>106014207</v>
       </c>
@@ -38866,7 +38863,7 @@
         <v>10395118</v>
       </c>
     </row>
-    <row r="398" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A398" s="4">
         <v>106334457</v>
       </c>
@@ -38952,7 +38949,7 @@
         <v>2866045</v>
       </c>
     </row>
-    <row r="399" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A399" s="4">
         <v>106444029</v>
       </c>
@@ -39038,7 +39035,7 @@
         <v>5600077</v>
       </c>
     </row>
-    <row r="400" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A400" s="4">
         <v>106504081</v>
       </c>
@@ -39124,7 +39121,7 @@
         <v>3042460</v>
       </c>
     </row>
-    <row r="401" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A401" s="4">
         <v>106014226</v>
       </c>
@@ -39210,7 +39207,7 @@
         <v>7653693</v>
       </c>
     </row>
-    <row r="402" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A402" s="4">
         <v>106334564</v>
       </c>
@@ -39296,7 +39293,7 @@
         <v>190506604</v>
       </c>
     </row>
-    <row r="403" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A403" s="4">
         <v>106400548</v>
       </c>
@@ -39382,7 +39379,7 @@
         <v>245702843</v>
       </c>
     </row>
-    <row r="404" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A404" s="4">
         <v>106330120</v>
       </c>
@@ -39468,7 +39465,7 @@
         <v>31019381</v>
       </c>
     </row>
-    <row r="405" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A405" s="4">
         <v>106191225</v>
       </c>
@@ -39554,7 +39551,7 @@
         <v>2894688</v>
       </c>
     </row>
-    <row r="406" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A406" s="4">
         <v>106190422</v>
       </c>
@@ -39640,7 +39637,7 @@
         <v>1238980352</v>
       </c>
     </row>
-    <row r="407" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A407" s="4">
         <v>106364451</v>
       </c>
@@ -39726,7 +39723,7 @@
         <v>8935224</v>
       </c>
     </row>
-    <row r="408" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A408" s="4">
         <v>106370780</v>
       </c>
@@ -39812,7 +39809,7 @@
         <v>246949276</v>
       </c>
     </row>
-    <row r="409" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A409" s="4">
         <v>106531059</v>
       </c>
@@ -39898,7 +39895,7 @@
         <v>27637008</v>
       </c>
     </row>
-    <row r="410" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A410" s="4">
         <v>106010776</v>
       </c>
@@ -39984,7 +39981,7 @@
         <v>925374528</v>
       </c>
     </row>
-    <row r="411" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A411" s="4">
         <v>106381154</v>
       </c>
@@ -40070,7 +40067,7 @@
         <v>8310081894</v>
       </c>
     </row>
-    <row r="412" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A412" s="4">
         <v>106341006</v>
       </c>
@@ -40156,7 +40153,7 @@
         <v>4703760497</v>
       </c>
     </row>
-    <row r="413" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A413" s="4">
         <v>106301279</v>
       </c>
@@ -40242,7 +40239,7 @@
         <v>3218524491</v>
       </c>
     </row>
-    <row r="414" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A414" s="4">
         <v>106370782</v>
       </c>
@@ -40328,7 +40325,7 @@
         <v>3758343109</v>
       </c>
     </row>
-    <row r="415" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A415" s="4">
         <v>106191216</v>
       </c>
@@ -40414,7 +40411,7 @@
         <v>247652786</v>
       </c>
     </row>
-    <row r="416" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A416" s="4">
         <v>106190818</v>
       </c>
@@ -40500,7 +40497,7 @@
         <v>82044598</v>
       </c>
     </row>
-    <row r="417" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A417" s="4">
         <v>106204019</v>
       </c>
@@ -40586,7 +40583,7 @@
         <v>2106397734</v>
       </c>
     </row>
-    <row r="418" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A418" s="4">
         <v>106190812</v>
       </c>
@@ -40672,7 +40669,7 @@
         <v>663962515</v>
       </c>
     </row>
-    <row r="419" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A419" s="4">
         <v>106014050</v>
       </c>
@@ -40758,7 +40755,7 @@
         <v>341971085</v>
       </c>
     </row>
-    <row r="420" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A420" s="4">
         <v>106560481</v>
       </c>
@@ -40844,7 +40841,7 @@
         <v>692305756</v>
       </c>
     </row>
-    <row r="421" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A421" s="4">
         <v>106454012</v>
       </c>
@@ -40930,7 +40927,7 @@
         <v>9602874</v>
       </c>
     </row>
-    <row r="422" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A422" s="4">
         <v>106344035</v>
       </c>
@@ -41016,7 +41013,7 @@
         <v>66955528</v>
       </c>
     </row>
-    <row r="423" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A423" s="4">
         <v>106334533</v>
       </c>
@@ -41102,7 +41099,7 @@
         <v>8488349</v>
       </c>
     </row>
-    <row r="424" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A424" s="4">
         <v>106361370</v>
       </c>
@@ -41188,7 +41185,7 @@
         <v>77732869</v>
       </c>
     </row>
-    <row r="425" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A425" s="4">
         <v>106010987</v>
       </c>
@@ -41274,7 +41271,7 @@
         <v>1294596308</v>
       </c>
     </row>
-    <row r="426" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A426" s="4">
         <v>106444013</v>
       </c>
@@ -41360,7 +41357,7 @@
         <v>85969166</v>
       </c>
     </row>
-    <row r="427" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A427" s="4">
         <v>106301379</v>
       </c>
@@ -41446,7 +41443,7 @@
         <v>176695285</v>
       </c>
     </row>
-    <row r="428" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A428" s="4">
         <v>106190857</v>
       </c>
@@ -41532,7 +41529,7 @@
         <v>9066566</v>
       </c>
     </row>
-    <row r="429" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A429" s="4">
         <v>106190859</v>
       </c>
@@ -41618,7 +41615,7 @@
         <v>1300459917</v>
       </c>
     </row>
-    <row r="430" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A430" s="4">
         <v>106190883</v>
       </c>
@@ -41704,7 +41701,7 @@
         <v>103756664</v>
       </c>
     </row>
-    <row r="431" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A431" s="4">
         <v>106571086</v>
       </c>
@@ -41790,7 +41787,7 @@
         <v>127384705</v>
       </c>
     </row>
-    <row r="432" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A432" s="4">
         <v>106380939</v>
       </c>
@@ -41877,8 +41874,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AD432" xr:uid="{0774DE2A-0243-434F-BFEB-08272A69030B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AB432">
+  <autoFilter ref="A1:AD432"/>
+  <sortState ref="A2:AB432">
     <sortCondition ref="B2:B432"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>